<commit_message>
Added a simple GUI using RayLib's Raygui
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -118,7 +118,7 @@
     <t>Bitprice</t>
   </si>
   <si>
-    <t>108.50</t>
+    <t>106.84</t>
   </si>
   <si>
     <t>https://www.skroutz.gr/shop/5426/Bitprice/products.html</t>
@@ -208,7 +208,7 @@
     <t>56.80</t>
   </si>
   <si>
-    <t>57.73</t>
+    <t>56.85</t>
   </si>
   <si>
     <t>57.97</t>
@@ -295,7 +295,7 @@
     <t>Emarket</t>
   </si>
   <si>
-    <t>84.50</t>
+    <t>82.50</t>
   </si>
   <si>
     <t>https://www.skroutz.gr/shop/14853/Emarket/products.html</t>

</xml_diff>